<commit_message>
Adicionando habilidades às profissoes
</commit_message>
<xml_diff>
--- a/docs/Profissoes.xlsx
+++ b/docs/Profissoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Gonçalves\Desktop\UVA\Monografia I\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Desktop\Projetos\monografia\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Banco de dados</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Analista de InfraEstrutura</t>
   </si>
   <si>
-    <t>Analista de testes</t>
-  </si>
-  <si>
     <t>Analista de Testes</t>
   </si>
   <si>
@@ -90,6 +87,18 @@
   </si>
   <si>
     <t>Redes</t>
+  </si>
+  <si>
+    <t>Acadêmico</t>
+  </si>
+  <si>
+    <t>Analista de redes</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Pesquisador</t>
   </si>
 </sst>
 </file>
@@ -197,16 +206,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,38 +501,41 @@
   <dimension ref="A1:AL57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="D1" sqref="D1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="1" max="2" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="11" max="11" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="L1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="P1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -546,20 +558,20 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
@@ -599,9 +611,11 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="P3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -635,9 +649,9 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
@@ -660,26 +674,26 @@
       <c r="AL4" s="3"/>
     </row>
     <row r="5" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="L5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
@@ -702,24 +716,24 @@
       <c r="AL5" s="3"/>
     </row>
     <row r="6" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="L6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="L6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -753,9 +767,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -789,9 +803,9 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -825,9 +839,9 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -861,9 +875,9 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -903,9 +917,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="P11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -939,9 +955,9 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -964,26 +980,24 @@
       <c r="AL12" s="3"/>
     </row>
     <row r="13" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="L13" s="6" t="s">
+      <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -1017,9 +1031,9 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1053,9 +1067,9 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
@@ -1089,9 +1103,9 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -1125,9 +1139,9 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
@@ -1157,7 +1171,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="3"/>
       <c r="H18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1165,9 +1179,9 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
@@ -1201,9 +1215,9 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
@@ -1230,16 +1244,18 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="H20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
@@ -1273,9 +1289,9 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
@@ -1309,9 +1325,9 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
@@ -1345,9 +1361,9 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
@@ -1383,9 +1399,9 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
@@ -1408,9 +1424,9 @@
       <c r="AL24" s="3"/>
     </row>
     <row r="25" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1419,9 +1435,9 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
@@ -1444,11 +1460,11 @@
       <c r="AL25" s="3"/>
     </row>
     <row r="26" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1457,9 +1473,9 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
@@ -1482,11 +1498,11 @@
       <c r="AL26" s="3"/>
     </row>
     <row r="27" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D27" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="D27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1495,9 +1511,9 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
@@ -1531,9 +1547,9 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
@@ -1567,9 +1583,9 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
@@ -1603,9 +1619,9 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
@@ -1639,9 +1655,9 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
@@ -1675,9 +1691,9 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
@@ -1711,9 +1727,9 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -1747,9 +1763,9 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
@@ -1783,9 +1799,9 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
@@ -1819,9 +1835,9 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
@@ -1855,9 +1871,9 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
@@ -1891,9 +1907,9 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
@@ -1927,9 +1943,9 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
@@ -1970,21 +1986,10 @@
     <row r="56" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="57" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="L3:N4"/>
-    <mergeCell ref="L11:N12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="H11:J12"/>
-    <mergeCell ref="H18:J19"/>
+  <mergeCells count="25">
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="P3:R4"/>
+    <mergeCell ref="P11:R12"/>
     <mergeCell ref="L1:N2"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D3:F4"/>
@@ -1993,6 +1998,20 @@
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D1:F2"/>
     <mergeCell ref="H1:J2"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D24:F25"/>
+    <mergeCell ref="L3:N4"/>
+    <mergeCell ref="L11:N12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="H11:J12"/>
+    <mergeCell ref="H18:J19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
criação de tela de pergunta e ajuste no background do site
</commit_message>
<xml_diff>
--- a/docs/Profissoes.xlsx
+++ b/docs/Profissoes.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Desktop\Projetos\monografia\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduser\Desktop\projetos\monografia\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Profissões" sheetId="1" r:id="rId1"/>
+    <sheet name="Habilidades" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Banco de dados</t>
   </si>
@@ -99,12 +100,57 @@
   </si>
   <si>
     <t>Pesquisador</t>
+  </si>
+  <si>
+    <t>Comunicativo</t>
+  </si>
+  <si>
+    <t>Criativo</t>
+  </si>
+  <si>
+    <t>Detalhista</t>
+  </si>
+  <si>
+    <t>Raciocínio Lógico</t>
+  </si>
+  <si>
+    <t>Solucionador</t>
+  </si>
+  <si>
+    <t>Organizado</t>
+  </si>
+  <si>
+    <t>Atencioso</t>
+  </si>
+  <si>
+    <t>Testador</t>
+  </si>
+  <si>
+    <t>Trabalho em equipe</t>
+  </si>
+  <si>
+    <t>Liderança</t>
+  </si>
+  <si>
+    <t>Investigador</t>
+  </si>
+  <si>
+    <t>Flexível</t>
+  </si>
+  <si>
+    <t>Pensamento Analítico</t>
+  </si>
+  <si>
+    <t>Preocupado com Segurança</t>
+  </si>
+  <si>
+    <t>Sensível ao próximo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,23 +247,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,7 +291,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -276,7 +329,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -348,7 +401,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,28 +567,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="L1" s="7" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -558,20 +611,20 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
@@ -674,26 +727,26 @@
       <c r="AL4" s="3"/>
     </row>
     <row r="5" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="L5" s="4" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="L5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
@@ -716,24 +769,24 @@
       <c r="AL5" s="3"/>
     </row>
     <row r="6" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -803,9 +856,9 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -839,9 +892,9 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -875,9 +928,9 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -980,17 +1033,17 @@
       <c r="AL12" s="3"/>
     </row>
     <row r="13" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1244,11 +1297,11 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1424,9 +1477,9 @@
       <c r="AL24" s="3"/>
     </row>
     <row r="25" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1460,11 +1513,11 @@
       <c r="AL25" s="3"/>
     </row>
     <row r="26" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1498,11 +1551,11 @@
       <c r="AL26" s="3"/>
     </row>
     <row r="27" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1986,19 +2039,7 @@
     <row r="56" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="57" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="P1:R2"/>
-    <mergeCell ref="P3:R4"/>
-    <mergeCell ref="P11:R12"/>
-    <mergeCell ref="L1:N2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="D11:F12"/>
-    <mergeCell ref="D18:F19"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="H1:J2"/>
-    <mergeCell ref="D26:F26"/>
+  <mergeCells count="30">
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D24:F25"/>
     <mergeCell ref="L3:N4"/>
@@ -2012,8 +2053,393 @@
     <mergeCell ref="H3:J4"/>
     <mergeCell ref="H11:J12"/>
     <mergeCell ref="H18:J19"/>
+    <mergeCell ref="D18:F19"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="H1:J2"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="P3:R4"/>
+    <mergeCell ref="P11:R12"/>
+    <mergeCell ref="L1:N2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="D11:F12"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P9:R9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="1.7109375" style="3" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="1.5703125" style="3" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="2.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="E6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="E7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="E8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="I8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="E10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="E11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="E12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="E13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="E14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="E4:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>